<commit_message>
增加 ExcelUtil getReader(String bookFilePath, String sheetName) 方法支持
</commit_message>
<xml_diff>
--- a/hutool-poi/src/test/resources/aaa.xlsx
+++ b/hutool-poi/src/test/resources/aaa.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1327A8C-2CEC-42B0-A8C4-49C104D61960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DDEAC3-B6E5-0C40-8D4F-DCB9F36BDAEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="13100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,13 +75,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -90,7 +90,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -233,7 +233,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -571,13 +571,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+    <sheetView zoomScale="193" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -591,7 +591,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -605,7 +605,7 @@
         <v>41.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -616,7 +616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
         <v>7</v>
@@ -641,9 +641,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -665,13 +665,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="226" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -685,7 +685,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -699,7 +699,7 @@
         <v>41.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -709,8 +709,11 @@
       <c r="C3" s="8">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
         <v>6</v>

</xml_diff>